<commit_message>
showing more details in trade-off analysis worksheet in excel
</commit_message>
<xml_diff>
--- a/MATLAB/results_tradeoff.xlsx
+++ b/MATLAB/results_tradeoff.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>AGV Model 1</t>
   </si>
@@ -164,6 +164,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,11 +210,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -227,6 +231,885 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Value Functions</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Alternatives!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AGV Model 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AGV Model 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AGV Model 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Alternatives!$K$3:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.60869565217391308</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66404410576333439</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65217391304347827</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AF0A-4B3B-B613-ACC7DD7E7B19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="482145488"/>
+        <c:axId val="437533840"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="482145488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="437533840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="437533840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="482145488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D69E72D-C839-4240-933D-044B6DE064FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D755678-9BDC-4043-936F-E1260256B598}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,12 +1426,12 @@
     <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -573,8 +1456,11 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,8 +1489,12 @@
         <f>SUM(C3:F3)*H3</f>
         <v>52000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" s="4">
+        <f>Calculations!I2</f>
+        <v>0.60869565217391308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,8 +1523,12 @@
         <f t="shared" ref="I4:I5" si="0">SUM(C4:F4)*H4</f>
         <v>84000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" s="4">
+        <f>Calculations!I3</f>
+        <v>0.66404410576333439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -663,13 +1557,17 @@
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5" s="4">
+        <f>Calculations!I4</f>
+        <v>0.65217391304347827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -693,7 +1591,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
         <v>0.04</v>
@@ -717,12 +1615,12 @@
         <v>550</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -730,7 +1628,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -738,7 +1636,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -766,6 +1664,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1049,7 +1948,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:R4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
small changes to trade-off analysis excel file
</commit_message>
<xml_diff>
--- a/MATLAB/results_tradeoff.xlsx
+++ b/MATLAB/results_tradeoff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{19B673CB-3D11-4D3D-881A-0B4E7398BD62}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{19B673CB-3D11-4D3D-881A-0B4E7398BD62}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternatives" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>AGV Model 1</t>
   </si>
@@ -346,13 +346,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.60869565217391308</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66404410576333439</c:v>
+                  <c:v>0.66878489685909392</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65217391304347827</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,15 +1076,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228601</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>142876</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1409,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D755678-9BDC-4043-936F-E1260256B598}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,6 +1424,7 @@
     <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1453,9 +1454,7 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="I2" s="1"/>
       <c r="K2" s="1" t="s">
         <v>35</v>
       </c>
@@ -1485,13 +1484,9 @@
       <c r="H3">
         <v>1000</v>
       </c>
-      <c r="I3">
-        <f>SUM(C3:F3)*H3</f>
-        <v>52000</v>
-      </c>
       <c r="K3" s="4">
         <f>Calculations!I2</f>
-        <v>0.60869565217391308</v>
+        <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1519,13 +1514,9 @@
       <c r="H4">
         <v>1500</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I5" si="0">SUM(C4:F4)*H4</f>
-        <v>84000</v>
-      </c>
       <c r="K4" s="4">
         <f>Calculations!I3</f>
-        <v>0.66404410576333439</v>
+        <v>0.66878489685909392</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1553,18 +1544,9 @@
       <c r="H5">
         <v>2000</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>120000</v>
-      </c>
       <c r="K5" s="4">
         <f>Calculations!I4</f>
-        <v>0.65217391304347827</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1592,7 +1574,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B9" s="2">
         <v>0.04</v>
       </c>
@@ -1615,50 +1599,60 @@
         <v>550</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="3" t="str">
-        <f>VLOOKUP(MAX(Calculations!I2:I4),Calculations!I2:J4,2,TRUE)</f>
+      <c r="B19" s="3" t="str">
+        <f>VLOOKUP(MAX(Calculations!I2:I4),Calculations!I2:J4,2,FALSE)</f>
         <v>AGV Model 2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1666,7 @@
           <x14:formula1>
             <xm:f>Calculations!$M$2:$M$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B20</xm:sqref>
+          <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1947,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A69C187-E67C-4B93-BDB6-7D13B4561F21}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:R4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2181,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2237,7 @@
         <v>0.75</v>
       </c>
       <c r="C2">
-        <f>Alternatives!I3</f>
+        <f>Alternatives!H3*SUM(Alternatives!C3:F3)</f>
         <v>52000</v>
       </c>
       <c r="D2">
@@ -2260,7 +2254,7 @@
       </c>
       <c r="I2">
         <f>($C$11*D2)+($C$12*E2)+($C$13*F2)</f>
-        <v>0.60869565217391308</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="J2" t="str">
         <f>Alternatives!A3</f>
@@ -2280,7 +2274,7 @@
         <v>0.75</v>
       </c>
       <c r="C3">
-        <f>Alternatives!I4</f>
+        <f>Alternatives!H4*SUM(Alternatives!C4:F4)</f>
         <v>84000</v>
       </c>
       <c r="D3">
@@ -2297,7 +2291,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I4" si="0">($C$11*D3)+($C$12*E3)+($C$13*F3)</f>
-        <v>0.66404410576333439</v>
+        <v>0.66878489685909392</v>
       </c>
       <c r="J3" t="str">
         <f>Alternatives!A4</f>
@@ -2317,7 +2311,7 @@
         <v>0.75</v>
       </c>
       <c r="C4">
-        <f>Alternatives!I5</f>
+        <f>Alternatives!H5*SUM(Alternatives!C5:F5)</f>
         <v>120000</v>
       </c>
       <c r="D4">
@@ -2334,7 +2328,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0.65217391304347827</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="J4" t="str">
         <f>Alternatives!A5</f>
@@ -2354,12 +2348,12 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <f>Alternatives!B12</f>
-        <v>90</v>
+        <f>Alternatives!B13</f>
+        <v>80</v>
       </c>
       <c r="C11">
         <f>B11/SUM($B$11:$B$13)</f>
-        <v>0.39130434782608697</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2367,12 +2361,12 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <f>Alternatives!B13</f>
+        <f>Alternatives!B14</f>
         <v>60</v>
       </c>
       <c r="C12">
         <f>B12/SUM($B$11:$B$13)</f>
-        <v>0.2608695652173913</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2380,12 +2374,12 @@
         <v>33</v>
       </c>
       <c r="B13">
-        <f>Alternatives!B14</f>
+        <f>Alternatives!B15</f>
         <v>80</v>
       </c>
       <c r="C13">
         <f>B13/SUM($B$11:$B$13)</f>
-        <v>0.34782608695652173</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>